<commit_message>
added extension delete test
</commit_message>
<xml_diff>
--- a/PM/src/main/java/testData/TestData.xlsx
+++ b/PM/src/main/java/testData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DE1B2C-E2C2-49D8-AB1D-8BBE1CFA6B0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05B7E1D-986F-42CF-B1EA-A9F08E115931}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -141,13 +141,22 @@
     <t>test_create_IP_extension</t>
   </si>
   <si>
-    <t>http://10.211.162.113/mp</t>
-  </si>
-  <si>
-    <t>http://10.211.162.113/wbm</t>
-  </si>
-  <si>
-    <t>number_initiate -number 77777..77779 -numbertype ex,77777-77779,77777,1,FirstName,LastName,Mitel 6869i</t>
+    <t>number_initiate -number 77777..77779 -numbertype ex,77777-77779,77777,1,FirstName,LastName,Mitel 6869i,ip_extension -e -d 77777,extension -e -d 77777,number_end -number 77777..77779 -numbertype ex</t>
+  </si>
+  <si>
+    <t>http://10.211.162.213/mp</t>
+  </si>
+  <si>
+    <t>http://10.211.162.213/wbm</t>
+  </si>
+  <si>
+    <t>test_delete_IP_extension</t>
+  </si>
+  <si>
+    <t>test_delete_multiple_IP_extension</t>
+  </si>
+  <si>
+    <t>number_initiate -number 70001..70010 -numbertype ex,extension -i -d 70001..70010 -l 1 --csp 0,ip_extension -i -d 70001..70010,70001-70010,ip_extension -e -d 70001..70010,extension -e -d 70001..70010,number_end -number 70001..70010 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -596,10 +605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECD1104-8824-4B0E-911A-8B0EFA495306}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,14 +746,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -794,7 +825,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,12 +835,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added edit ip extension to configure parallel ringing.
</commit_message>
<xml_diff>
--- a/PM/src/main/java/testData/TestData.xlsx
+++ b/PM/src/main/java/testData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mallikar\git\PM\PM\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05B7E1D-986F-42CF-B1EA-A9F08E115931}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1C90E1-7CC6-45CD-8D73-5B8DDFE9F081}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Arjuna,Arjuna@12345</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>number_initiate -number 70001..70010 -numbertype ex,extension -i -d 70001..70010 -l 1 --csp 0,ip_extension -i -d 70001..70010,70001-70010,ip_extension -e -d 70001..70010,extension -e -d 70001..70010,number_end -number 70001..70010 -numbertype ex</t>
+  </si>
+  <si>
+    <t>test_configureParallel_ringing_to_IP</t>
+  </si>
+  <si>
+    <t>number_initiate -number 70001..70003 -numbertype ex,extension -i -d 70001..70003 -l 1 --csp 0,ip_extension -i -d 70001..70003,70001-70003,70001,70002,70003,parallel_ringing -e -d 70001,ip_extension -e -d 70001..70003,extension -e -d 70001..70003,number_end -number 70001..70003 -numbertype ex</t>
   </si>
 </sst>
 </file>
@@ -605,10 +611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECD1104-8824-4B0E-911A-8B0EFA495306}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,6 +782,17 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>